<commit_message>
Assetliste, Zeiterfassung, 3D Assets
</commit_message>
<xml_diff>
--- a/_Artbible/Assetliste.xlsx
+++ b/_Artbible/Assetliste.xlsx
@@ -825,9 +825,6 @@
     <t>Tür 200cm höhe / 100cm breit</t>
   </si>
   <si>
-    <t>100cm breit/100cm tief</t>
-  </si>
-  <si>
     <t>Müss man Öffnen können</t>
   </si>
   <si>
@@ -835,6 +832,9 @@
   </si>
   <si>
     <t>Mülleimer</t>
+  </si>
+  <si>
+    <t>100cm breit/100cm tief/5cm dick</t>
   </si>
 </sst>
 </file>
@@ -1430,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="K69" sqref="K69"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="61" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B61" s="27"/>
       <c r="C61" s="27"/>
@@ -3314,7 +3314,7 @@
       <c r="H109" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I109" s="5"/>
+      <c r="I109" s="18"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
@@ -3480,7 +3480,7 @@
       <c r="H121" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I121" s="17"/>
+      <c r="I121" s="18"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="6"/>
@@ -3496,12 +3496,12 @@
         <v>268</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H122" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I122" s="5"/>
+      <c r="I122" s="17"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="6"/>
@@ -3548,13 +3548,13 @@
         <v>144</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="G125" s="3"/>
       <c r="H125" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I125" s="5"/>
+      <c r="I125" s="18"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="6"/>
@@ -3567,13 +3567,13 @@
         <v>145</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="G126" s="3"/>
       <c r="H126" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I126" s="5"/>
+      <c r="I126" s="18"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">

</xml_diff>

<commit_message>
Assets & Asset Liste
</commit_message>
<xml_diff>
--- a/_Artbible/Assetliste.xlsx
+++ b/_Artbible/Assetliste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="273">
   <si>
     <t>Nummer</t>
   </si>
@@ -135,21 +135,12 @@
     <t>Seitenteil groß</t>
   </si>
   <si>
-    <t>160cm höhe/ 40cm tief</t>
-  </si>
-  <si>
     <t>Seitenteil klein</t>
   </si>
   <si>
-    <t>200cm höhe/ 40cm tief</t>
-  </si>
-  <si>
     <t>Regalboden groß</t>
   </si>
   <si>
-    <t>200cm breit/ 40 cm tief</t>
-  </si>
-  <si>
     <t>120cm breit/ 60cm tiefe</t>
   </si>
   <si>
@@ -162,9 +153,6 @@
     <t>Regalboden klein</t>
   </si>
   <si>
-    <t>100cm breit/ 40cm tief</t>
-  </si>
-  <si>
     <t>Modular</t>
   </si>
   <si>
@@ -835,6 +823,18 @@
   </si>
   <si>
     <t>100cm breit/100cm tief/5cm dick</t>
+  </si>
+  <si>
+    <t>160cm höhe/ 40cm tief/8cm dick</t>
+  </si>
+  <si>
+    <t>200cm höhe/ 40cm tief/8cm dick</t>
+  </si>
+  <si>
+    <t>200cm breit/ 40 cm tief/8cm dick</t>
+  </si>
+  <si>
+    <t>100cm breit/ 40cm tief/8cm dick</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1038,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1067,6 +1067,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20 % - Akzent1" xfId="4" builtinId="30"/>
@@ -1430,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="I109" sqref="I109"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>1</v>
@@ -1481,16 +1483,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="13" t="s">
@@ -1506,11 +1508,11 @@
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1521,7 +1523,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N3" s="15"/>
     </row>
@@ -1533,7 +1535,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1546,7 +1548,7 @@
         <v>4</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="N4" s="15"/>
     </row>
@@ -1558,7 +1560,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -1569,19 +1571,19 @@
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="18" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N5" s="15"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -1604,7 +1606,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -1627,7 +1629,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -1652,7 +1654,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -1675,7 +1677,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -1700,7 +1702,7 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -1738,10 +1740,10 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="10" t="s">
@@ -1750,10 +1752,10 @@
       <c r="I13" s="5"/>
       <c r="K13" s="15"/>
       <c r="L13" s="22" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N13" s="15"/>
     </row>
@@ -1765,7 +1767,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1775,10 +1777,10 @@
       <c r="I14" s="5"/>
       <c r="K14" s="15"/>
       <c r="L14" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="N14" s="15"/>
     </row>
@@ -1790,7 +1792,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1800,7 +1802,7 @@
       <c r="I15" s="5"/>
       <c r="K15" s="15"/>
       <c r="L15" s="22" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="M15" s="22" t="s">
         <v>9</v>
@@ -1810,12 +1812,12 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1825,7 +1827,7 @@
       <c r="I16" s="5"/>
       <c r="K16" s="15"/>
       <c r="L16" s="22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="M16" s="22" t="s">
         <v>10</v>
@@ -1840,7 +1842,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -1850,7 +1852,7 @@
       <c r="I17" s="5"/>
       <c r="K17" s="15"/>
       <c r="L17" s="22" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="M17" s="22" t="s">
         <v>11</v>
@@ -1865,7 +1867,7 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -1875,10 +1877,10 @@
       <c r="I18" s="5"/>
       <c r="K18" s="15"/>
       <c r="L18" s="22" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="N18" s="15"/>
     </row>
@@ -1890,7 +1892,7 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1900,10 +1902,10 @@
       <c r="I19" s="5"/>
       <c r="K19" s="15"/>
       <c r="L19" s="22" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N19" s="15"/>
     </row>
@@ -1919,26 +1921,26 @@
       <c r="I20" s="2"/>
       <c r="K20" s="15"/>
       <c r="L20" s="22" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="N20" s="15"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="5"/>
@@ -1971,12 +1973,14 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="I23" s="5"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1992,10 +1996,10 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G24" s="3"/>
       <c r="I24" s="5"/>
@@ -2013,7 +2017,7 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>31</v>
@@ -2071,7 +2075,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>36</v>
@@ -2109,13 +2113,13 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="5"/>
@@ -2144,10 +2148,12 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
@@ -2157,65 +2163,73 @@
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>39</v>
+        <v>270</v>
       </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="5"/>
+      <c r="H33" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>41</v>
+        <v>269</v>
       </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="5"/>
+      <c r="H34" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>43</v>
+        <v>271</v>
       </c>
       <c r="G35" s="3"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="5"/>
+      <c r="H35" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>48</v>
+        <v>272</v>
       </c>
       <c r="G36" s="3"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="5"/>
+      <c r="H36" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" s="18"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -2230,16 +2244,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="2"/>
@@ -2258,19 +2272,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="5"/>
@@ -2288,16 +2302,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G42" s="7"/>
       <c r="H42" s="2"/>
@@ -2316,16 +2330,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
       <c r="E44" s="11" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="2"/>
@@ -2344,7 +2358,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -2359,14 +2373,14 @@
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="2"/>
@@ -2376,14 +2390,14 @@
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="11" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G48" s="11"/>
       <c r="H48" s="2"/>
@@ -2393,14 +2407,14 @@
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="2"/>
@@ -2410,17 +2424,17 @@
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="5"/>
@@ -2429,14 +2443,14 @@
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="2"/>
@@ -2446,14 +2460,14 @@
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="2"/>
@@ -2463,14 +2477,14 @@
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D53" s="11"/>
       <c r="E53" s="11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="2"/>
@@ -2480,14 +2494,14 @@
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D54" s="11"/>
       <c r="E54" s="11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G54" s="11"/>
       <c r="H54" s="2"/>
@@ -2497,14 +2511,14 @@
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="2"/>
@@ -2523,16 +2537,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="2"/>
@@ -2551,16 +2565,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="24" t="s">
@@ -2581,7 +2595,7 @@
     </row>
     <row r="61" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B61" s="27"/>
       <c r="C61" s="27"/>
@@ -2605,7 +2619,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -2620,14 +2634,14 @@
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="11" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G64" s="11"/>
       <c r="H64" s="2"/>
@@ -2637,11 +2651,11 @@
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D65" s="11"/>
       <c r="E65" s="11" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
@@ -2661,16 +2675,16 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G67" s="11"/>
       <c r="H67" s="2"/>
@@ -2689,7 +2703,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -2704,14 +2718,14 @@
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D70" s="11"/>
       <c r="E70" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G70" s="11"/>
       <c r="H70" s="2"/>
@@ -2721,14 +2735,14 @@
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D71" s="11"/>
       <c r="E71" s="11" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G71" s="11"/>
       <c r="H71" s="2"/>
@@ -2738,14 +2752,14 @@
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D72" s="11"/>
       <c r="E72" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G72" s="11"/>
       <c r="H72" s="2"/>
@@ -2764,7 +2778,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -2779,15 +2793,15 @@
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="5"/>
@@ -2796,11 +2810,11 @@
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
@@ -2811,11 +2825,11 @@
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
@@ -2826,11 +2840,11 @@
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
@@ -2841,11 +2855,11 @@
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
@@ -2856,11 +2870,11 @@
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
@@ -2871,11 +2885,11 @@
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
@@ -2886,11 +2900,11 @@
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
@@ -2901,15 +2915,15 @@
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -2918,11 +2932,11 @@
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D84" s="11"/>
       <c r="E84" s="11" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F84" s="11"/>
       <c r="G84" s="11"/>
@@ -2933,11 +2947,11 @@
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D85" s="11"/>
       <c r="E85" s="11" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F85" s="11"/>
       <c r="G85" s="11"/>
@@ -2948,11 +2962,11 @@
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="11" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D86" s="11"/>
       <c r="E86" s="11" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F86" s="11"/>
       <c r="G86" s="11"/>
@@ -2972,16 +2986,16 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="7" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G88" s="7"/>
       <c r="H88" s="2"/>
@@ -3000,7 +3014,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
@@ -3015,14 +3029,14 @@
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G91" s="11"/>
       <c r="H91" s="2"/>
@@ -3032,14 +3046,14 @@
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D92" s="11"/>
       <c r="E92" s="11" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G92" s="11"/>
       <c r="H92" s="2"/>
@@ -3049,14 +3063,14 @@
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D93" s="11"/>
       <c r="E93" s="11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F93" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G93" s="11"/>
       <c r="H93" s="2"/>
@@ -3066,14 +3080,14 @@
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D94" s="11"/>
       <c r="E94" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G94" s="11"/>
       <c r="H94" s="2"/>
@@ -3083,14 +3097,14 @@
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D95" s="11"/>
       <c r="E95" s="11" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G95" s="11"/>
       <c r="H95" s="2"/>
@@ -3100,14 +3114,14 @@
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F96" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G96" s="11"/>
       <c r="H96" s="2"/>
@@ -3117,14 +3131,14 @@
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D97" s="11"/>
       <c r="E97" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F97" s="11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G97" s="11"/>
       <c r="H97" s="2"/>
@@ -3134,14 +3148,14 @@
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D98" s="11"/>
       <c r="E98" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G98" s="11"/>
       <c r="H98" s="2"/>
@@ -3160,7 +3174,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B100" s="11"/>
       <c r="C100" s="11"/>
@@ -3175,14 +3189,14 @@
       <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="C101" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D101" s="11"/>
       <c r="E101" s="11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F101" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G101" s="11"/>
       <c r="H101" s="2"/>
@@ -3192,15 +3206,15 @@
       <c r="A102" s="6"/>
       <c r="B102" s="6"/>
       <c r="C102" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D102" s="11"/>
       <c r="E102" s="11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F102" s="11"/>
       <c r="G102" s="11" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="5"/>
@@ -3209,15 +3223,15 @@
       <c r="A103" s="6"/>
       <c r="B103" s="6"/>
       <c r="C103" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D103" s="11"/>
       <c r="E103" s="11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F103" s="11"/>
       <c r="G103" s="11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="5"/>
@@ -3226,15 +3240,15 @@
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D104" s="11"/>
       <c r="E104" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F104" s="11"/>
       <c r="G104" s="11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H104" s="2"/>
       <c r="I104" s="5"/>
@@ -3243,15 +3257,15 @@
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
       <c r="F105" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G105" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H105" s="2"/>
       <c r="I105" s="5"/>
@@ -3269,7 +3283,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -3284,14 +3298,14 @@
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D108" s="9"/>
       <c r="E108" s="9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G108" s="9"/>
       <c r="H108" s="2"/>
@@ -3301,14 +3315,14 @@
       <c r="A109" s="2"/>
       <c r="B109" s="6"/>
       <c r="C109" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G109" s="3"/>
       <c r="H109" s="24" t="s">
@@ -3320,14 +3334,14 @@
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D110" s="9"/>
       <c r="E110" s="9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G110" s="9"/>
       <c r="H110" s="2"/>
@@ -3346,17 +3360,17 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F112" s="11"/>
       <c r="G112" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H112" s="6"/>
       <c r="I112" s="5"/>
@@ -3374,7 +3388,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -3398,13 +3412,13 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
@@ -3424,16 +3438,16 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B118" s="11"/>
       <c r="C118" s="11"/>
       <c r="D118" s="11"/>
       <c r="E118" s="11" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F118" s="11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G118" s="11"/>
       <c r="H118" s="6"/>
@@ -3452,7 +3466,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -3467,14 +3481,14 @@
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D121" s="3"/>
       <c r="E121" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G121" s="3"/>
       <c r="H121" s="24" t="s">
@@ -3486,17 +3500,17 @@
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H122" s="24" t="s">
         <v>23</v>
@@ -3507,14 +3521,14 @@
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G123" s="3"/>
       <c r="H123" s="6"/>
@@ -3524,14 +3538,14 @@
       <c r="A124" s="6"/>
       <c r="B124" s="6"/>
       <c r="C124" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G124" s="3"/>
       <c r="H124" s="6"/>
@@ -3541,14 +3555,14 @@
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="C125" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D125" s="3"/>
       <c r="E125" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G125" s="3"/>
       <c r="H125" s="24" t="s">
@@ -3560,14 +3574,14 @@
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
       <c r="C126" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G126" s="3"/>
       <c r="H126" s="24" t="s">
@@ -3577,7 +3591,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -3592,7 +3606,7 @@
       <c r="A128" s="6"/>
       <c r="B128" s="6"/>
       <c r="C128" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
@@ -3605,7 +3619,7 @@
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="C129" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>

</xml_diff>

<commit_message>
Assets, Assetliste & Zeiterfassung
</commit_message>
<xml_diff>
--- a/_Artbible/Assetliste.xlsx
+++ b/_Artbible/Assetliste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="273">
   <si>
     <t>Nummer</t>
   </si>
@@ -486,9 +486,6 @@
     <t>Kiste mittel</t>
   </si>
   <si>
-    <t>Kiste Groß</t>
-  </si>
-  <si>
     <t>65cm höhe</t>
   </si>
   <si>
@@ -835,6 +832,9 @@
   </si>
   <si>
     <t>100cm breit/ 40cm tief/8cm dick</t>
+  </si>
+  <si>
+    <t>Kiste groß</t>
   </si>
 </sst>
 </file>
@@ -1432,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J106" sqref="J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,13 +1483,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>74</v>
@@ -1508,11 +1508,11 @@
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1535,7 +1535,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1560,7 +1560,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -1578,12 +1578,12 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -1606,7 +1606,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -1629,7 +1629,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -1654,7 +1654,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -1677,7 +1677,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -1702,7 +1702,7 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -1740,7 +1740,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>75</v>
@@ -1767,7 +1767,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1792,7 +1792,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1812,12 +1812,12 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1842,7 +1842,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -1867,7 +1867,7 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -1892,7 +1892,7 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1930,17 +1930,17 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="5"/>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>41</v>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>31</v>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>36</v>
@@ -2113,7 +2113,7 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>42</v>
@@ -2163,10 +2163,10 @@
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="29" t="s">
@@ -2182,10 +2182,10 @@
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="24" t="s">
@@ -2201,10 +2201,10 @@
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="24" t="s">
@@ -2220,10 +2220,10 @@
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="24" t="s">
@@ -2244,16 +2244,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>235</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="2"/>
@@ -2278,7 +2278,7 @@
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>48</v>
@@ -2308,7 +2308,7 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>52</v>
@@ -2336,7 +2336,7 @@
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
       <c r="E44" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F44" s="11" t="s">
         <v>54</v>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>113</v>
@@ -2390,14 +2390,14 @@
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G48" s="11"/>
       <c r="H48" s="2"/>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>112</v>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F50" s="11" t="s">
         <v>114</v>
@@ -2447,7 +2447,7 @@
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>118</v>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F52" s="11" t="s">
         <v>113</v>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="D53" s="11"/>
       <c r="E53" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>121</v>
@@ -2498,7 +2498,7 @@
       </c>
       <c r="D54" s="11"/>
       <c r="E54" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>123</v>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>125</v>
@@ -2543,7 +2543,7 @@
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>94</v>
@@ -2571,7 +2571,7 @@
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>95</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="61" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B61" s="27"/>
       <c r="C61" s="27"/>
@@ -2619,7 +2619,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -2634,11 +2634,11 @@
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F64" s="11" t="s">
         <v>131</v>
@@ -2651,11 +2651,11 @@
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D65" s="11"/>
       <c r="E65" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
@@ -2681,7 +2681,7 @@
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F67" s="11" t="s">
         <v>96</v>
@@ -2722,7 +2722,7 @@
       </c>
       <c r="D70" s="11"/>
       <c r="E70" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F70" s="11" t="s">
         <v>79</v>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="D71" s="11"/>
       <c r="E71" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F71" s="11" t="s">
         <v>80</v>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="D72" s="11"/>
       <c r="E72" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F72" s="11" t="s">
         <v>81</v>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7" t="s">
@@ -2814,7 +2814,7 @@
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
@@ -2870,11 +2870,11 @@
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
@@ -2915,15 +2915,15 @@
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -2932,11 +2932,11 @@
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D84" s="11"/>
       <c r="E84" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F84" s="11"/>
       <c r="G84" s="11"/>
@@ -2947,11 +2947,11 @@
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D85" s="11"/>
       <c r="E85" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F85" s="11"/>
       <c r="G85" s="11"/>
@@ -2962,11 +2962,11 @@
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D86" s="11"/>
       <c r="E86" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F86" s="11"/>
       <c r="G86" s="11"/>
@@ -2986,16 +2986,16 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="F88" s="7" t="s">
         <v>246</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>247</v>
       </c>
       <c r="G88" s="7"/>
       <c r="H88" s="2"/>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F91" s="11" t="s">
         <v>82</v>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="D92" s="11"/>
       <c r="E92" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F92" s="11" t="s">
         <v>82</v>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="D93" s="11"/>
       <c r="E93" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F93" s="11" t="s">
         <v>83</v>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="D94" s="11"/>
       <c r="E94" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F94" s="11" t="s">
         <v>83</v>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="D95" s="11"/>
       <c r="E95" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F95" s="11" t="s">
         <v>84</v>
@@ -3118,7 +3118,7 @@
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F96" s="11" t="s">
         <v>84</v>
@@ -3135,7 +3135,7 @@
       </c>
       <c r="D97" s="11"/>
       <c r="E97" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F97" s="11" t="s">
         <v>85</v>
@@ -3152,7 +3152,7 @@
       </c>
       <c r="D98" s="11"/>
       <c r="E98" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F98" s="11" t="s">
         <v>85</v>
@@ -3193,7 +3193,7 @@
       </c>
       <c r="D101" s="11"/>
       <c r="E101" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F101" s="11" t="s">
         <v>97</v>
@@ -3210,11 +3210,11 @@
       </c>
       <c r="D102" s="11"/>
       <c r="E102" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F102" s="11"/>
       <c r="G102" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="5"/>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="D103" s="11"/>
       <c r="E103" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F103" s="11"/>
       <c r="G103" s="11" t="s">
@@ -3244,7 +3244,7 @@
       </c>
       <c r="D104" s="11"/>
       <c r="E104" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F104" s="11"/>
       <c r="G104" s="11" t="s">
@@ -3291,8 +3291,10 @@
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
-      <c r="H107" s="6"/>
-      <c r="I107" s="5"/>
+      <c r="H107" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I107" s="18"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
@@ -3302,14 +3304,16 @@
       </c>
       <c r="D108" s="9"/>
       <c r="E108" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G108" s="9"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="5"/>
+      <c r="H108" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I108" s="18"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
@@ -3319,7 +3323,7 @@
       </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F109" s="3" t="s">
         <v>74</v>
@@ -3334,18 +3338,20 @@
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="9" t="s">
-        <v>156</v>
+        <v>272</v>
       </c>
       <c r="D110" s="9"/>
       <c r="E110" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G110" s="9"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="5"/>
+      <c r="H110" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I110" s="18"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
@@ -3366,7 +3372,7 @@
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F112" s="11"/>
       <c r="G112" s="11" t="s">
@@ -3418,7 +3424,7 @@
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
@@ -3444,7 +3450,7 @@
       <c r="C118" s="11"/>
       <c r="D118" s="11"/>
       <c r="E118" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F118" s="11" t="s">
         <v>126</v>
@@ -3488,7 +3494,7 @@
         <v>138</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G121" s="3"/>
       <c r="H121" s="24" t="s">
@@ -3507,48 +3513,52 @@
         <v>137</v>
       </c>
       <c r="F122" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="G122" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="G122" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="H122" s="24" t="s">
+      <c r="H122" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I122" s="17"/>
+      <c r="I122" s="18"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3" t="s">
         <v>136</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G123" s="3"/>
-      <c r="H123" s="6"/>
+      <c r="H123" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="I123" s="5"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="6"/>
       <c r="B124" s="6"/>
       <c r="C124" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3" t="s">
         <v>139</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G124" s="3"/>
-      <c r="H124" s="6"/>
+      <c r="H124" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="I124" s="5"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -3562,7 +3572,7 @@
         <v>140</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G125" s="3"/>
       <c r="H125" s="24" t="s">
@@ -3581,7 +3591,7 @@
         <v>141</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G126" s="3"/>
       <c r="H126" s="24" t="s">
@@ -3591,7 +3601,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -3606,7 +3616,7 @@
       <c r="A128" s="6"/>
       <c r="B128" s="6"/>
       <c r="C128" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
@@ -3619,7 +3629,7 @@
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="C129" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>

</xml_diff>

<commit_message>
Assetliste, Ready to Implement
</commit_message>
<xml_diff>
--- a/_Artbible/Assetliste.xlsx
+++ b/_Artbible/Assetliste.xlsx
@@ -1432,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J106" sqref="J106"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3481,7 +3481,7 @@
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="H120" s="6"/>
-      <c r="I120" s="5"/>
+      <c r="I120" s="18"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="6"/>
@@ -3540,7 +3540,7 @@
       <c r="H123" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I123" s="5"/>
+      <c r="I123" s="18"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="6"/>
@@ -3559,7 +3559,7 @@
       <c r="H124" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I124" s="5"/>
+      <c r="I124" s="18"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/ArtjomProGrammer/Voodoo"
This reverts commit d0c1d7877fba3bc78b9544f638d35bec32683c3f, reversing
changes made to 97091328e61cd694c6ededd9ff1194a8ab80e3e3.
</commit_message>
<xml_diff>
--- a/_Artbible/Assetliste.xlsx
+++ b/_Artbible/Assetliste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="273">
   <si>
     <t>Nummer</t>
   </si>
@@ -135,12 +135,21 @@
     <t>Seitenteil groß</t>
   </si>
   <si>
+    <t>160cm höhe/ 40cm tief</t>
+  </si>
+  <si>
     <t>Seitenteil klein</t>
   </si>
   <si>
+    <t>200cm höhe/ 40cm tief</t>
+  </si>
+  <si>
     <t>Regalboden groß</t>
   </si>
   <si>
+    <t>200cm breit/ 40 cm tief</t>
+  </si>
+  <si>
     <t>120cm breit/ 60cm tiefe</t>
   </si>
   <si>
@@ -153,6 +162,9 @@
     <t>Regalboden klein</t>
   </si>
   <si>
+    <t>100cm breit/ 40cm tief</t>
+  </si>
+  <si>
     <t>Modular</t>
   </si>
   <si>
@@ -486,6 +498,9 @@
     <t>Kiste mittel</t>
   </si>
   <si>
+    <t>Kiste Groß</t>
+  </si>
+  <si>
     <t>65cm höhe</t>
   </si>
   <si>
@@ -820,21 +835,6 @@
   </si>
   <si>
     <t>100cm breit/100cm tief/5cm dick</t>
-  </si>
-  <si>
-    <t>160cm höhe/ 40cm tief/8cm dick</t>
-  </si>
-  <si>
-    <t>200cm höhe/ 40cm tief/8cm dick</t>
-  </si>
-  <si>
-    <t>200cm breit/ 40 cm tief/8cm dick</t>
-  </si>
-  <si>
-    <t>100cm breit/ 40cm tief/8cm dick</t>
-  </si>
-  <si>
-    <t>Kiste groß</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1038,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1067,8 +1067,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20 % - Akzent1" xfId="4" builtinId="30"/>
@@ -1432,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>1</v>
@@ -1483,16 +1481,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="13" t="s">
@@ -1508,11 +1506,11 @@
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1523,7 +1521,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N3" s="15"/>
     </row>
@@ -1535,7 +1533,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1548,7 +1546,7 @@
         <v>4</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="N4" s="15"/>
     </row>
@@ -1560,7 +1558,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -1571,19 +1569,19 @@
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="18" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="N5" s="15"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -1606,7 +1604,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -1629,7 +1627,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -1654,7 +1652,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -1677,7 +1675,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -1702,7 +1700,7 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -1740,10 +1738,10 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="10" t="s">
@@ -1752,10 +1750,10 @@
       <c r="I13" s="5"/>
       <c r="K13" s="15"/>
       <c r="L13" s="22" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N13" s="15"/>
     </row>
@@ -1767,7 +1765,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1777,10 +1775,10 @@
       <c r="I14" s="5"/>
       <c r="K14" s="15"/>
       <c r="L14" s="22" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="N14" s="15"/>
     </row>
@@ -1792,7 +1790,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1802,7 +1800,7 @@
       <c r="I15" s="5"/>
       <c r="K15" s="15"/>
       <c r="L15" s="22" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M15" s="22" t="s">
         <v>9</v>
@@ -1812,12 +1810,12 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1827,7 +1825,7 @@
       <c r="I16" s="5"/>
       <c r="K16" s="15"/>
       <c r="L16" s="22" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="M16" s="22" t="s">
         <v>10</v>
@@ -1842,7 +1840,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -1852,7 +1850,7 @@
       <c r="I17" s="5"/>
       <c r="K17" s="15"/>
       <c r="L17" s="22" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="M17" s="22" t="s">
         <v>11</v>
@@ -1867,7 +1865,7 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -1877,10 +1875,10 @@
       <c r="I18" s="5"/>
       <c r="K18" s="15"/>
       <c r="L18" s="22" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="N18" s="15"/>
     </row>
@@ -1892,7 +1890,7 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1902,10 +1900,10 @@
       <c r="I19" s="5"/>
       <c r="K19" s="15"/>
       <c r="L19" s="22" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="N19" s="15"/>
     </row>
@@ -1921,26 +1919,26 @@
       <c r="I20" s="2"/>
       <c r="K20" s="15"/>
       <c r="L20" s="22" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="N20" s="15"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="5"/>
@@ -1973,14 +1971,12 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="28" t="s">
-        <v>23</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="H23" s="2"/>
       <c r="I23" s="5"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1996,16 +1992,13 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G24" s="3"/>
-      <c r="H24" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="18"/>
+      <c r="I24" s="5"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -2020,7 +2013,7 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>31</v>
@@ -2028,10 +2021,8 @@
       <c r="G25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" s="17"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="5"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2080,7 +2071,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>36</v>
@@ -2118,13 +2109,13 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="5"/>
@@ -2153,12 +2144,10 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H32" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="18"/>
+        <v>49</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
@@ -2168,73 +2157,65 @@
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>269</v>
+        <v>39</v>
       </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I33" s="18"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>268</v>
+        <v>41</v>
       </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I34" s="18"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>270</v>
+        <v>43</v>
       </c>
       <c r="G35" s="3"/>
-      <c r="H35" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I35" s="18"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>271</v>
+        <v>48</v>
       </c>
       <c r="G36" s="3"/>
-      <c r="H36" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I36" s="18"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -2249,16 +2230,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="2"/>
@@ -2277,19 +2258,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="5"/>
@@ -2307,16 +2288,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G42" s="7"/>
       <c r="H42" s="2"/>
@@ -2335,16 +2316,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
       <c r="E44" s="11" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="2"/>
@@ -2363,7 +2344,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -2378,14 +2359,14 @@
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="2"/>
@@ -2395,14 +2376,14 @@
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="11" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="G48" s="11"/>
       <c r="H48" s="2"/>
@@ -2412,14 +2393,14 @@
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="7" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="2"/>
@@ -2429,17 +2410,17 @@
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="11" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="11" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="5"/>
@@ -2448,14 +2429,14 @@
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="11" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="2"/>
@@ -2465,14 +2446,14 @@
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="11" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="11" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="2"/>
@@ -2482,14 +2463,14 @@
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="11" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D53" s="11"/>
       <c r="E53" s="11" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="2"/>
@@ -2499,14 +2480,14 @@
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="11" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D54" s="11"/>
       <c r="E54" s="11" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="G54" s="11"/>
       <c r="H54" s="2"/>
@@ -2516,14 +2497,14 @@
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="11" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="11" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="2"/>
@@ -2542,16 +2523,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="2"/>
@@ -2570,16 +2551,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="24" t="s">
@@ -2600,7 +2581,7 @@
     </row>
     <row r="61" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B61" s="27"/>
       <c r="C61" s="27"/>
@@ -2624,7 +2605,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -2639,14 +2620,14 @@
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="11" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="11" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="G64" s="11"/>
       <c r="H64" s="2"/>
@@ -2656,11 +2637,11 @@
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="11" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="D65" s="11"/>
       <c r="E65" s="11" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
@@ -2680,16 +2661,16 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G67" s="11"/>
       <c r="H67" s="2"/>
@@ -2708,7 +2689,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -2723,14 +2704,14 @@
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="11" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D70" s="11"/>
       <c r="E70" s="11" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="G70" s="11"/>
       <c r="H70" s="2"/>
@@ -2740,14 +2721,14 @@
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D71" s="11"/>
       <c r="E71" s="11" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G71" s="11"/>
       <c r="H71" s="2"/>
@@ -2757,14 +2738,14 @@
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="11" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D72" s="11"/>
       <c r="E72" s="11" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G72" s="11"/>
       <c r="H72" s="2"/>
@@ -2783,7 +2764,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -2798,15 +2779,15 @@
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="7" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="5"/>
@@ -2815,11 +2796,11 @@
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="7" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
@@ -2830,11 +2811,11 @@
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="7" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
@@ -2845,11 +2826,11 @@
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="7" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
@@ -2860,11 +2841,11 @@
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="7" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
@@ -2875,11 +2856,11 @@
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="7" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="7" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
@@ -2890,11 +2871,11 @@
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
@@ -2905,11 +2886,11 @@
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="7" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
@@ -2920,15 +2901,15 @@
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="7" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -2937,11 +2918,11 @@
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="11" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D84" s="11"/>
       <c r="E84" s="11" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="F84" s="11"/>
       <c r="G84" s="11"/>
@@ -2952,11 +2933,11 @@
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="11" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="D85" s="11"/>
       <c r="E85" s="11" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="F85" s="11"/>
       <c r="G85" s="11"/>
@@ -2967,11 +2948,11 @@
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="11" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D86" s="11"/>
       <c r="E86" s="11" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="F86" s="11"/>
       <c r="G86" s="11"/>
@@ -2991,16 +2972,16 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="7" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="G88" s="7"/>
       <c r="H88" s="2"/>
@@ -3019,7 +3000,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
@@ -3034,14 +3015,14 @@
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="11" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="11" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G91" s="11"/>
       <c r="H91" s="2"/>
@@ -3051,14 +3032,14 @@
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D92" s="11"/>
       <c r="E92" s="11" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G92" s="11"/>
       <c r="H92" s="2"/>
@@ -3068,14 +3049,14 @@
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="11" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D93" s="11"/>
       <c r="E93" s="11" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="F93" s="11" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G93" s="11"/>
       <c r="H93" s="2"/>
@@ -3085,14 +3066,14 @@
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="11" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D94" s="11"/>
       <c r="E94" s="11" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G94" s="11"/>
       <c r="H94" s="2"/>
@@ -3102,14 +3083,14 @@
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="11" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D95" s="11"/>
       <c r="E95" s="11" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G95" s="11"/>
       <c r="H95" s="2"/>
@@ -3119,14 +3100,14 @@
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="F96" s="11" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G96" s="11"/>
       <c r="H96" s="2"/>
@@ -3136,14 +3117,14 @@
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="11" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D97" s="11"/>
       <c r="E97" s="11" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="F97" s="11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G97" s="11"/>
       <c r="H97" s="2"/>
@@ -3153,14 +3134,14 @@
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="11" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D98" s="11"/>
       <c r="E98" s="11" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G98" s="11"/>
       <c r="H98" s="2"/>
@@ -3179,7 +3160,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B100" s="11"/>
       <c r="C100" s="11"/>
@@ -3194,14 +3175,14 @@
       <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="C101" s="11" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D101" s="11"/>
       <c r="E101" s="11" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="F101" s="11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G101" s="11"/>
       <c r="H101" s="2"/>
@@ -3211,15 +3192,15 @@
       <c r="A102" s="6"/>
       <c r="B102" s="6"/>
       <c r="C102" s="11" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D102" s="11"/>
       <c r="E102" s="11" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="F102" s="11"/>
       <c r="G102" s="11" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="5"/>
@@ -3228,15 +3209,15 @@
       <c r="A103" s="6"/>
       <c r="B103" s="6"/>
       <c r="C103" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D103" s="11"/>
       <c r="E103" s="11" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="F103" s="11"/>
       <c r="G103" s="11" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="5"/>
@@ -3245,15 +3226,15 @@
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="11" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D104" s="11"/>
       <c r="E104" s="11" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="F104" s="11"/>
       <c r="G104" s="11" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="H104" s="2"/>
       <c r="I104" s="5"/>
@@ -3262,15 +3243,15 @@
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="11" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
       <c r="F105" s="11" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G105" s="11" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H105" s="2"/>
       <c r="I105" s="5"/>
@@ -3288,7 +3269,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -3296,42 +3277,38 @@
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
-      <c r="H107" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I107" s="18"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="5"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="9" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D108" s="9"/>
       <c r="E108" s="9" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="G108" s="9"/>
-      <c r="H108" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I108" s="18"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="5"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="6"/>
       <c r="C109" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G109" s="3"/>
       <c r="H109" s="24" t="s">
@@ -3343,20 +3320,18 @@
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="9" t="s">
-        <v>272</v>
+        <v>160</v>
       </c>
       <c r="D110" s="9"/>
       <c r="E110" s="9" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="G110" s="9"/>
-      <c r="H110" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I110" s="18"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="5"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
@@ -3371,17 +3346,17 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="F112" s="11"/>
       <c r="G112" s="11" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="H112" s="6"/>
       <c r="I112" s="5"/>
@@ -3399,7 +3374,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -3423,13 +3398,13 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="7" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
@@ -3449,16 +3424,16 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B118" s="11"/>
       <c r="C118" s="11"/>
       <c r="D118" s="11"/>
       <c r="E118" s="11" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F118" s="11" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G118" s="11"/>
       <c r="H118" s="6"/>
@@ -3477,7 +3452,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -3486,20 +3461,20 @@
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="H120" s="6"/>
-      <c r="I120" s="18"/>
+      <c r="I120" s="5"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D121" s="3"/>
       <c r="E121" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="G121" s="3"/>
       <c r="H121" s="24" t="s">
@@ -3511,73 +3486,69 @@
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="H122" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="H122" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I122" s="18"/>
+      <c r="I122" s="17"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="G123" s="3"/>
-      <c r="H123" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I123" s="18"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="5"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="6"/>
       <c r="B124" s="6"/>
       <c r="C124" s="3" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="G124" s="3"/>
-      <c r="H124" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I124" s="18"/>
+      <c r="H124" s="6"/>
+      <c r="I124" s="5"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="C125" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D125" s="3"/>
       <c r="E125" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="G125" s="3"/>
       <c r="H125" s="24" t="s">
@@ -3589,14 +3560,14 @@
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
       <c r="C126" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="G126" s="3"/>
       <c r="H126" s="24" t="s">
@@ -3606,7 +3577,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -3621,7 +3592,7 @@
       <c r="A128" s="6"/>
       <c r="B128" s="6"/>
       <c r="C128" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
@@ -3634,7 +3605,7 @@
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="C129" s="3" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>

</xml_diff>

<commit_message>
Assetliste, Assets und Zeiterfassung
</commit_message>
<xml_diff>
--- a/_Artbible/Assetliste.xlsx
+++ b/_Artbible/Assetliste.xlsx
@@ -1277,7 +1277,7 @@
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1346,7 +1346,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="10" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20 % - Akzent1" xfId="1" builtinId="30"/>
@@ -2543,8 +2542,8 @@
   </sheetPr>
   <dimension ref="A1:IV175"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G155" sqref="G155"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I139" sqref="I139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -6108,7 +6107,7 @@
       <c r="H139" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="I139" s="68"/>
+      <c r="I139" s="61"/>
       <c r="J139" s="58"/>
       <c r="K139" s="58"/>
       <c r="L139" s="58"/>

</xml_diff>